<commit_message>
Fixed Issues in Test Scripts
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/TestData/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/TestData/FreeCRMTestData.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Tasks" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:L13"/>
 </workbook>
 </file>
 
@@ -430,6 +429,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">

</xml_diff>